<commit_message>
ab regression updates + preprocessing
</commit_message>
<xml_diff>
--- a/deloitte_digital_banking/data/Account Products.xlsx
+++ b/deloitte_digital_banking/data/Account Products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbennett/Documents/bse/term3/masters_thesis/Deloitte/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbennett/Documents/bse/term3/deloitte_digital_banking/deloitte_digital_banking/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2E0BD6-4FAF-A14E-96B6-43252AF4DC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A176F1CF-EF10-A247-8AE7-D3AC74E8F06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" activeTab="5" xr2:uid="{7E25AA3E-10FA-4F11-A62D-B7563CA3921C}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="2" xr2:uid="{7E25AA3E-10FA-4F11-A62D-B7563CA3921C}"/>
   </bookViews>
   <sheets>
     <sheet name="account_products" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="611">
   <si>
     <t>account product</t>
   </si>
@@ -1838,118 +1838,10 @@
     <t>Best Comission-Free Accounts (Helmycash)</t>
   </si>
   <si>
-    <t>Cuenta Online sin comisiones BBVA</t>
-  </si>
-  <si>
-    <t>Cuenta Nómina ING </t>
-  </si>
-  <si>
-    <t>Cuenta Nómina hasta 5% TAE Bankinter</t>
-  </si>
-  <si>
-    <t>Cuenta Clara ABANCA</t>
-  </si>
-  <si>
-    <t>Cuenta Online SIN Liberbank</t>
-  </si>
-  <si>
-    <t>Cuenta Corriente Open Openbank</t>
-  </si>
-  <si>
-    <t>Cuenta imagin</t>
-  </si>
-  <si>
-    <t>Cuenta Inteligente Bienvenida EVO Banco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuenta Online Banco Sabadell </t>
-  </si>
-  <si>
-    <t>Cuenta Online Banco Santander</t>
-  </si>
-  <si>
-    <t>Cuenta No Cuenta ING</t>
-  </si>
-  <si>
     <t>Best Salary Accounts (Helmycash)</t>
   </si>
   <si>
-    <t>Cuenta Nómina Open Openbank</t>
-  </si>
-  <si>
-    <t>Cuenta Nómina Va Contigo BBVA</t>
-  </si>
-  <si>
-    <t>Cuenta imagin con Nómina</t>
-  </si>
-  <si>
-    <t>Cuenta Inteligente Bienvenida Nómina EVO Banco</t>
-  </si>
-  <si>
-    <t>Cuenta Nómina Sin Comisiones BBVA</t>
-  </si>
-  <si>
     <t>Best Savings Accounts (Helpmycash)</t>
-  </si>
-  <si>
-    <t>Cuenta Expansión Plus Sabadell</t>
-  </si>
-  <si>
-    <t>Cuenta de Ahorro Bienvenida con Nómina Openbank</t>
-  </si>
-  <si>
-    <t>Cuenta Evolución Banco Mediolanum</t>
-  </si>
-  <si>
-    <t>Cuenta 2% MyInvestor</t>
-  </si>
-  <si>
-    <t>Cuenta Ahorro Orange Bank</t>
-  </si>
-  <si>
-    <t>Cuenta Contigo Renault Bank</t>
-  </si>
-  <si>
-    <t>Cuenta Remunerada Pibank</t>
-  </si>
-  <si>
-    <t>Cuenta de Ahorro Online Nationale Nederlanden</t>
-  </si>
-  <si>
-    <t>Cuenta de Ahorro Progretto</t>
-  </si>
-  <si>
-    <t>Cuenta Naranja ING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cuenta de Ahorro BraBank </t>
-  </si>
-  <si>
-    <t>Cuenta PlayStation Unicaja Banco</t>
-  </si>
-  <si>
-    <t>Cuenta de Ahorro Bank Norwegian</t>
-  </si>
-  <si>
-    <t>Cuenta de Ahorro Klarna</t>
-  </si>
-  <si>
-    <t>Cuenta Vamos Ibercaja</t>
-  </si>
-  <si>
-    <t>Cuenta Día a Día Caixabank</t>
-  </si>
-  <si>
-    <t>Cuenta MoneyGo</t>
-  </si>
-  <si>
-    <t>Cuenta Remunerada Scalable Capital</t>
-  </si>
-  <si>
-    <t>Cuenta Remunerada EBAN Banco</t>
-  </si>
-  <si>
-    <t>Cuenta de Ahorro Distingo Bank</t>
   </si>
   <si>
     <t>Date</t>
@@ -2129,6 +2021,45 @@
   </si>
   <si>
     <t>age of bank</t>
+  </si>
+  <si>
+    <t>BankInter</t>
+  </si>
+  <si>
+    <t>Abanca</t>
+  </si>
+  <si>
+    <t>Liberbank</t>
+  </si>
+  <si>
+    <t>N26.com</t>
+  </si>
+  <si>
+    <t>Imagin</t>
+  </si>
+  <si>
+    <t>EVOBanco</t>
+  </si>
+  <si>
+    <t>BancoSabadell</t>
+  </si>
+  <si>
+    <t>BancoSantander</t>
+  </si>
+  <si>
+    <t>OrangeBank</t>
+  </si>
+  <si>
+    <t>RenaultBank</t>
+  </si>
+  <si>
+    <t>PiBank</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>CaixaBank</t>
   </si>
 </sst>
 </file>
@@ -7063,8 +6994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F329555A-7C3C-43C8-ADA4-B5A5C7DC827F}">
   <dimension ref="A2:AB61"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="136" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:AB12"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="136" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7179,7 +7110,7 @@
         <v>540</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>541</v>
+        <v>19</v>
       </c>
       <c r="C9" s="32">
         <v>1</v>
@@ -7247,7 +7178,7 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="62"/>
       <c r="B10" t="s">
-        <v>542</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -7286,7 +7217,7 @@
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="62"/>
       <c r="B11" t="s">
-        <v>543</v>
+        <v>598</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -7319,7 +7250,7 @@
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="62"/>
       <c r="B12" t="s">
-        <v>544</v>
+        <v>599</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -7376,7 +7307,7 @@
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="62"/>
       <c r="B13" t="s">
-        <v>545</v>
+        <v>600</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -7397,7 +7328,7 @@
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="62"/>
       <c r="B14" t="s">
-        <v>546</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -7457,7 +7388,7 @@
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="62"/>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>601</v>
       </c>
       <c r="C15">
         <v>7</v>
@@ -7517,7 +7448,7 @@
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="62"/>
       <c r="B16" t="s">
-        <v>547</v>
+        <v>602</v>
       </c>
       <c r="C16">
         <v>8</v>
@@ -7541,7 +7472,7 @@
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="62"/>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17">
         <v>6</v>
@@ -7592,7 +7523,7 @@
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="62"/>
       <c r="B18" t="s">
-        <v>548</v>
+        <v>603</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -7628,7 +7559,7 @@
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="62"/>
       <c r="B19" t="s">
-        <v>549</v>
+        <v>604</v>
       </c>
       <c r="K19">
         <v>2</v>
@@ -7670,7 +7601,7 @@
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="62"/>
       <c r="B20" t="s">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="K20">
         <v>6</v>
@@ -7712,7 +7643,7 @@
     <row r="21" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="63"/>
       <c r="B21" s="4" t="s">
-        <v>551</v>
+        <v>16</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -7759,10 +7690,10 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="64" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>543</v>
+        <v>598</v>
       </c>
       <c r="C22" s="32">
         <v>1</v>
@@ -7810,7 +7741,7 @@
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="65"/>
       <c r="B23" t="s">
-        <v>542</v>
+        <v>16</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -7870,7 +7801,7 @@
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="65"/>
       <c r="B24" t="s">
-        <v>553</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -7918,7 +7849,7 @@
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="65"/>
       <c r="B25" t="s">
-        <v>544</v>
+        <v>599</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -7975,7 +7906,7 @@
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="65"/>
       <c r="B26" t="s">
-        <v>554</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -8029,7 +7960,7 @@
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="65"/>
       <c r="B27" t="s">
-        <v>545</v>
+        <v>600</v>
       </c>
       <c r="C27">
         <v>6</v>
@@ -8050,7 +7981,7 @@
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="65"/>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>601</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -8107,7 +8038,7 @@
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="65"/>
       <c r="B29" t="s">
-        <v>555</v>
+        <v>602</v>
       </c>
       <c r="H29">
         <v>8</v>
@@ -8122,7 +8053,7 @@
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="65"/>
       <c r="B30" t="s">
-        <v>556</v>
+        <v>603</v>
       </c>
       <c r="I30">
         <v>4</v>
@@ -8155,7 +8086,7 @@
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="65"/>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>604</v>
       </c>
       <c r="K31">
         <v>5</v>
@@ -8197,7 +8128,7 @@
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="65"/>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>605</v>
       </c>
       <c r="K32">
         <v>6</v>
@@ -8239,7 +8170,7 @@
     <row r="33" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="66"/>
       <c r="B33" s="4" t="s">
-        <v>557</v>
+        <v>19</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -8276,10 +8207,10 @@
     </row>
     <row r="34" spans="1:28" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="58" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>543</v>
+        <v>598</v>
       </c>
       <c r="C34" s="32">
         <v>1</v>
@@ -8347,7 +8278,7 @@
     <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="59"/>
       <c r="B35" t="s">
-        <v>559</v>
+        <v>604</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -8374,7 +8305,7 @@
     <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="59"/>
       <c r="B36" t="s">
-        <v>560</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -8434,7 +8365,7 @@
     <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="59"/>
       <c r="B37" t="s">
-        <v>561</v>
+        <v>603</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -8467,7 +8398,7 @@
     <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="59"/>
       <c r="B38" t="s">
-        <v>562</v>
+        <v>34</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -8515,7 +8446,7 @@
     <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="59"/>
       <c r="B39" t="s">
-        <v>563</v>
+        <v>606</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -8551,7 +8482,7 @@
     <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="59"/>
       <c r="B40" t="s">
-        <v>564</v>
+        <v>607</v>
       </c>
       <c r="C40">
         <v>7</v>
@@ -8602,7 +8533,7 @@
     <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="59"/>
       <c r="B41" t="s">
-        <v>565</v>
+        <v>608</v>
       </c>
       <c r="C41">
         <v>8</v>
@@ -8638,7 +8569,7 @@
     <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="59"/>
       <c r="B42" t="s">
-        <v>566</v>
+        <v>609</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -8665,7 +8596,7 @@
     <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="59"/>
       <c r="B43" t="s">
-        <v>567</v>
+        <v>609</v>
       </c>
       <c r="C43">
         <v>10</v>
@@ -8704,7 +8635,7 @@
     <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="59"/>
       <c r="B44" t="s">
-        <v>568</v>
+        <v>16</v>
       </c>
       <c r="C44">
         <v>11</v>
@@ -8725,7 +8656,7 @@
     <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="59"/>
       <c r="B45" t="s">
-        <v>569</v>
+        <v>609</v>
       </c>
       <c r="I45">
         <v>10</v>
@@ -8737,7 +8668,7 @@
     <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="59"/>
       <c r="B46" t="s">
-        <v>453</v>
+        <v>609</v>
       </c>
       <c r="J46">
         <v>9</v>
@@ -8773,7 +8704,7 @@
     <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="59"/>
       <c r="B47" t="s">
-        <v>570</v>
+        <v>609</v>
       </c>
       <c r="K47">
         <v>2</v>
@@ -8797,7 +8728,7 @@
     <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="59"/>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>604</v>
       </c>
       <c r="K48">
         <v>5</v>
@@ -8835,7 +8766,7 @@
     <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="59"/>
       <c r="B49" t="s">
-        <v>571</v>
+        <v>609</v>
       </c>
       <c r="N49">
         <v>10</v>
@@ -8862,7 +8793,7 @@
     <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="59"/>
       <c r="B50" t="s">
-        <v>572</v>
+        <v>609</v>
       </c>
       <c r="O50">
         <v>10</v>
@@ -8877,7 +8808,7 @@
     <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="59"/>
       <c r="B51" t="s">
-        <v>425</v>
+        <v>609</v>
       </c>
       <c r="Q51">
         <v>8</v>
@@ -8898,7 +8829,7 @@
     <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="59"/>
       <c r="B52" t="s">
-        <v>573</v>
+        <v>609</v>
       </c>
       <c r="Q52">
         <v>1</v>
@@ -8919,7 +8850,7 @@
     <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="59"/>
       <c r="B53" t="s">
-        <v>574</v>
+        <v>610</v>
       </c>
       <c r="Q53">
         <v>2</v>
@@ -8934,7 +8865,7 @@
     <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="59"/>
       <c r="B54" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
       <c r="Q54">
         <v>3</v>
@@ -8961,7 +8892,7 @@
     <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="59"/>
       <c r="B55" t="s">
-        <v>576</v>
+        <v>609</v>
       </c>
       <c r="R55">
         <v>6</v>
@@ -8979,7 +8910,7 @@
     <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="59"/>
       <c r="B56" t="s">
-        <v>544</v>
+        <v>599</v>
       </c>
       <c r="R56">
         <v>8</v>
@@ -8991,7 +8922,7 @@
     <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="59"/>
       <c r="B57" t="s">
-        <v>548</v>
+        <v>603</v>
       </c>
       <c r="V57">
         <v>8</v>
@@ -9012,7 +8943,7 @@
     <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="59"/>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>601</v>
       </c>
       <c r="V58">
         <v>10</v>
@@ -9027,7 +8958,7 @@
     <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="59"/>
       <c r="B59" t="s">
-        <v>577</v>
+        <v>609</v>
       </c>
       <c r="Z59" s="35">
         <v>9</v>
@@ -9038,7 +8969,7 @@
     <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="59"/>
       <c r="B60" t="s">
-        <v>506</v>
+        <v>609</v>
       </c>
       <c r="Z60" s="35"/>
       <c r="AA60" s="35">
@@ -9049,7 +8980,7 @@
     <row r="61" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="60"/>
       <c r="B61" s="4" t="s">
-        <v>578</v>
+        <v>609</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -9109,7 +9040,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>579</v>
+        <v>543</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>11</v>
@@ -9145,7 +9076,7 @@
         <v>17</v>
       </c>
       <c r="M1" s="46" t="s">
-        <v>580</v>
+        <v>544</v>
       </c>
       <c r="N1" s="46" t="s">
         <v>26</v>
@@ -10179,7 +10110,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="67" t="s">
-        <v>581</v>
+        <v>545</v>
       </c>
       <c r="C1" s="67"/>
       <c r="D1" s="67"/>
@@ -10201,49 +10132,49 @@
         <v>47</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>582</v>
+        <v>546</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>583</v>
+        <v>547</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>584</v>
+        <v>548</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>585</v>
+        <v>549</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>586</v>
+        <v>550</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>587</v>
+        <v>551</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>588</v>
+        <v>552</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>589</v>
+        <v>553</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>590</v>
+        <v>554</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>591</v>
+        <v>555</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>592</v>
+        <v>556</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>593</v>
+        <v>557</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>594</v>
+        <v>558</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>595</v>
+        <v>559</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>596</v>
+        <v>560</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -11459,8 +11390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE22D15A-8004-7B41-B711-BA4B1E533A45}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11472,28 +11403,28 @@
   <sheetData>
     <row r="1" spans="1:16" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
-        <v>630</v>
+        <v>594</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>631</v>
+        <v>595</v>
       </c>
       <c r="C1" s="48" t="s">
+        <v>561</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>562</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>563</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>564</v>
+      </c>
+      <c r="G1" s="48" t="s">
         <v>597</v>
       </c>
-      <c r="D1" s="48" t="s">
-        <v>598</v>
-      </c>
-      <c r="E1" s="48" t="s">
-        <v>599</v>
-      </c>
-      <c r="F1" s="48" t="s">
-        <v>600</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>633</v>
-      </c>
       <c r="H1" s="48" t="s">
-        <v>632</v>
+        <v>596</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -11507,7 +11438,7 @@
     <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="47"/>
       <c r="B2" s="48" t="s">
-        <v>582</v>
+        <v>546</v>
       </c>
       <c r="C2" s="48">
         <v>5946</v>
@@ -11523,7 +11454,7 @@
         <v>2011</v>
       </c>
       <c r="H2" s="47" t="s">
-        <v>629</v>
+        <v>593</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -11537,7 +11468,7 @@
     <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="47"/>
       <c r="B3" s="48" t="s">
-        <v>583</v>
+        <v>547</v>
       </c>
       <c r="C3" s="48">
         <v>212764</v>
@@ -11553,16 +11484,16 @@
         <v>1857</v>
       </c>
       <c r="H3" s="47" t="s">
-        <v>626</v>
+        <v>590</v>
       </c>
       <c r="I3" t="s">
-        <v>602</v>
+        <v>566</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="47"/>
       <c r="B4" s="48" t="s">
-        <v>584</v>
+        <v>548</v>
       </c>
       <c r="C4" s="48">
         <v>19316</v>
@@ -11578,16 +11509,16 @@
         <v>1881</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>601</v>
+        <v>565</v>
       </c>
       <c r="I4" t="s">
-        <v>603</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="48" t="s">
-        <v>585</v>
+        <v>549</v>
       </c>
       <c r="C5" s="48">
         <v>6138</v>
@@ -11603,19 +11534,19 @@
         <v>1965</v>
       </c>
       <c r="H5" s="47" t="s">
-        <v>605</v>
+        <v>569</v>
       </c>
       <c r="I5" t="s">
-        <v>606</v>
+        <v>570</v>
       </c>
       <c r="J5" t="s">
-        <v>607</v>
+        <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="47"/>
       <c r="B6" s="48" t="s">
-        <v>586</v>
+        <v>550</v>
       </c>
       <c r="C6" s="48">
         <v>121486</v>
@@ -11631,16 +11562,16 @@
         <v>1857</v>
       </c>
       <c r="H6" s="47" t="s">
-        <v>601</v>
+        <v>565</v>
       </c>
       <c r="I6" t="s">
-        <v>604</v>
+        <v>568</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="47"/>
       <c r="B7" s="48" t="s">
-        <v>587</v>
+        <v>551</v>
       </c>
       <c r="C7" s="48">
         <v>44863</v>
@@ -11656,19 +11587,19 @@
         <v>1904</v>
       </c>
       <c r="H7" s="47" t="s">
-        <v>601</v>
+        <v>565</v>
       </c>
       <c r="I7" t="s">
-        <v>608</v>
+        <v>572</v>
       </c>
       <c r="J7" t="s">
-        <v>609</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="47"/>
       <c r="B8" s="48" t="s">
-        <v>588</v>
+        <v>552</v>
       </c>
       <c r="C8" s="48">
         <v>200</v>
@@ -11684,21 +11615,21 @@
         <v>2012</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>610</v>
+        <v>574</v>
       </c>
       <c r="I8" t="s">
-        <v>611</v>
+        <v>575</v>
       </c>
       <c r="J8" t="s">
-        <v>612</v>
+        <v>576</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
-        <v>614</v>
+        <v>578</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>589</v>
+        <v>553</v>
       </c>
       <c r="C9" s="48">
         <v>118</v>
@@ -11716,13 +11647,13 @@
         <v>2016</v>
       </c>
       <c r="H9" s="47" t="s">
-        <v>613</v>
+        <v>577</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="47"/>
       <c r="B10" s="48" t="s">
-        <v>590</v>
+        <v>554</v>
       </c>
       <c r="C10" s="48">
         <v>60778</v>
@@ -11740,16 +11671,16 @@
         <v>1991</v>
       </c>
       <c r="H10" s="47" t="s">
-        <v>615</v>
+        <v>579</v>
       </c>
       <c r="I10" t="s">
-        <v>616</v>
+        <v>580</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="47"/>
       <c r="B11" s="48" t="s">
-        <v>591</v>
+        <v>555</v>
       </c>
       <c r="C11" s="48">
         <v>5343</v>
@@ -11765,19 +11696,19 @@
         <v>2012</v>
       </c>
       <c r="H11" s="47" t="s">
-        <v>617</v>
+        <v>581</v>
       </c>
       <c r="I11" t="s">
-        <v>618</v>
+        <v>582</v>
       </c>
       <c r="J11" t="s">
-        <v>619</v>
+        <v>583</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="47"/>
       <c r="B12" s="48" t="s">
-        <v>592</v>
+        <v>556</v>
       </c>
       <c r="C12" s="48">
         <v>60</v>
@@ -11793,16 +11724,16 @@
         <v>2017</v>
       </c>
       <c r="H12" s="47" t="s">
-        <v>620</v>
+        <v>584</v>
       </c>
       <c r="I12" t="s">
-        <v>621</v>
+        <v>585</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="47"/>
       <c r="B13" s="48" t="s">
-        <v>593</v>
+        <v>557</v>
       </c>
       <c r="C13" s="48">
         <v>1500</v>
@@ -11818,18 +11749,18 @@
         <v>2013</v>
       </c>
       <c r="H13" s="47" t="s">
-        <v>622</v>
+        <v>586</v>
       </c>
       <c r="I13" t="s">
-        <v>623</v>
+        <v>587</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="47" t="s">
-        <v>624</v>
+        <v>588</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>594</v>
+        <v>558</v>
       </c>
       <c r="C14" s="48">
         <v>1100</v>
@@ -11845,19 +11776,21 @@
         <v>1996</v>
       </c>
       <c r="H14" s="47" t="s">
-        <v>625</v>
+        <v>589</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="47"/>
       <c r="B15" s="48" t="s">
-        <v>595</v>
+        <v>559</v>
       </c>
       <c r="C15" s="48">
         <v>65</v>
       </c>
       <c r="D15" s="47"/>
-      <c r="E15" s="49"/>
+      <c r="E15" s="49">
+        <v>15500000000</v>
+      </c>
       <c r="F15" s="47">
         <v>0</v>
       </c>
@@ -11865,13 +11798,13 @@
         <v>2018</v>
       </c>
       <c r="H15" s="47" t="s">
-        <v>627</v>
+        <v>591</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="47"/>
       <c r="B16" s="48" t="s">
-        <v>596</v>
+        <v>560</v>
       </c>
       <c r="C16" s="48">
         <v>7500</v>
@@ -11887,7 +11820,7 @@
         <v>2015</v>
       </c>
       <c r="H16" s="47" t="s">
-        <v>628</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -11896,29 +11829,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8a57f42c-87cf-45dc-a824-f519bec23429" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6364f5f1-3e58-4c48-b30e-88ea54b7be43">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="8a57f42c-87cf-45dc-a824-f519bec23429">
-      <UserInfo>
-        <DisplayName>Real, Carlos</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Caceres Arconada, Natalia</DisplayName>
-        <AccountId>24</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A385B01D1FD0014E944A5E4F345173E4" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a3771546bd7ab637c8273a988636753c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6364f5f1-3e58-4c48-b30e-88ea54b7be43" xmlns:ns3="8a57f42c-87cf-45dc-a824-f519bec23429" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="313d26ddbc9013adaf4e24971c4c3998" ns2:_="" ns3:_="">
     <xsd:import namespace="6364f5f1-3e58-4c48-b30e-88ea54b7be43"/>
@@ -12153,6 +12063,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8a57f42c-87cf-45dc-a824-f519bec23429" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6364f5f1-3e58-4c48-b30e-88ea54b7be43">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="8a57f42c-87cf-45dc-a824-f519bec23429">
+      <UserInfo>
+        <DisplayName>Real, Carlos</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Caceres Arconada, Natalia</DisplayName>
+        <AccountId>24</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12163,17 +12096,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{374B9168-07C8-4BD4-B7BC-5E948D43D7EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8a57f42c-87cf-45dc-a824-f519bec23429"/>
-    <ds:schemaRef ds:uri="6364f5f1-3e58-4c48-b30e-88ea54b7be43"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E860F67E-69A3-4AF4-9748-74E66B4DD00E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12192,6 +12114,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{374B9168-07C8-4BD4-B7BC-5E948D43D7EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8a57f42c-87cf-45dc-a824-f519bec23429"/>
+    <ds:schemaRef ds:uri="6364f5f1-3e58-4c48-b30e-88ea54b7be43"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD12C9DB-3EE9-4235-AEF0-FD3713628091}">
   <ds:schemaRefs>

</xml_diff>